<commit_message>
AJout SD dans le pinconfig et dans le HSIS
</commit_message>
<xml_diff>
--- a/ApaliPi_Config.xlsx
+++ b/ApaliPi_Config.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="12" documentId="11_7D32F1691DB66D67231ED9CB4688A30A4BC6AC1F" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F0EE940D-88D5-4466-B3C9-1E278B8A5929}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B11A89-82D2-4BEB-9A7C-AB044FE2769B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="345" windowWidth="16605" windowHeight="13755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1035" yWindow="1155" windowWidth="16605" windowHeight="13755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pin Configuration" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="264">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="285">
   <si>
     <t>Signal</t>
   </si>
@@ -807,13 +807,76 @@
   </si>
   <si>
     <t>USB3_DN</t>
+  </si>
+  <si>
+    <t>SD_1_CD#</t>
+  </si>
+  <si>
+    <t>GPIO-CC.05</t>
+  </si>
+  <si>
+    <t>CLK2_REQ</t>
+  </si>
+  <si>
+    <t>SD_1_CLK</t>
+  </si>
+  <si>
+    <t>SDMMC1-SCLK</t>
+  </si>
+  <si>
+    <t>SDMMC1_CLK</t>
+  </si>
+  <si>
+    <t>SD_1_CMD</t>
+  </si>
+  <si>
+    <t>SDMMC1-CMD</t>
+  </si>
+  <si>
+    <t>SDMMC1_CMD</t>
+  </si>
+  <si>
+    <t>SD_1_D0</t>
+  </si>
+  <si>
+    <t>SDMMC1-DAT0</t>
+  </si>
+  <si>
+    <t>SDMMC1_DAT0</t>
+  </si>
+  <si>
+    <t>SD_1_D1</t>
+  </si>
+  <si>
+    <t>SDMMC1-DAT1</t>
+  </si>
+  <si>
+    <t>SDMMC1_DAT1</t>
+  </si>
+  <si>
+    <t>SD_1_D2</t>
+  </si>
+  <si>
+    <t>SDMMC1-DAT2</t>
+  </si>
+  <si>
+    <t>SDMMC1_DAT2</t>
+  </si>
+  <si>
+    <t>SD_1_D3</t>
+  </si>
+  <si>
+    <t>SDMMC1-DAT3</t>
+  </si>
+  <si>
+    <t>SDMMC1_DAT3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -838,6 +901,19 @@
       <sz val="11"/>
       <color rgb="FF27BD4B"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF27BD4B"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -893,7 +969,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -926,6 +1002,14 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1270,10 +1354,10 @@
   <sheetPr>
     <tabColor rgb="FFFC0000"/>
   </sheetPr>
-  <dimension ref="A1:J72"/>
+  <dimension ref="A1:J79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A67" sqref="A67"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="D87" sqref="D87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3381,6 +3465,176 @@
         <v>76</v>
       </c>
     </row>
+    <row r="73" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A73" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="B73" s="7">
+        <v>190</v>
+      </c>
+      <c r="C73" s="7"/>
+      <c r="D73" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="E73" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F73" s="7"/>
+      <c r="G73" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="H73" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="I73" s="14"/>
+      <c r="J73" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A74" s="6" t="s">
+        <v>267</v>
+      </c>
+      <c r="B74" s="10">
+        <v>184</v>
+      </c>
+      <c r="C74" s="10"/>
+      <c r="D74" s="10" t="s">
+        <v>268</v>
+      </c>
+      <c r="E74" s="10"/>
+      <c r="F74" s="10"/>
+      <c r="G74" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H74" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="I74" s="16"/>
+      <c r="J74" s="17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A75" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="B75" s="7">
+        <v>180</v>
+      </c>
+      <c r="C75" s="7"/>
+      <c r="D75" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="E75" s="7"/>
+      <c r="F75" s="7"/>
+      <c r="G75" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H75" s="7" t="s">
+        <v>272</v>
+      </c>
+      <c r="I75" s="14"/>
+      <c r="J75" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A76" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="B76" s="10">
+        <v>186</v>
+      </c>
+      <c r="C76" s="10"/>
+      <c r="D76" s="10" t="s">
+        <v>274</v>
+      </c>
+      <c r="E76" s="10"/>
+      <c r="F76" s="10"/>
+      <c r="G76" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H76" s="10" t="s">
+        <v>275</v>
+      </c>
+      <c r="I76" s="16"/>
+      <c r="J76" s="17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A77" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="B77" s="7">
+        <v>188</v>
+      </c>
+      <c r="C77" s="7"/>
+      <c r="D77" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="E77" s="7"/>
+      <c r="F77" s="7"/>
+      <c r="G77" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H77" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="I77" s="14"/>
+      <c r="J77" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A78" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="B78" s="10">
+        <v>176</v>
+      </c>
+      <c r="C78" s="10"/>
+      <c r="D78" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="E78" s="10"/>
+      <c r="F78" s="10"/>
+      <c r="G78" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="H78" s="10" t="s">
+        <v>281</v>
+      </c>
+      <c r="I78" s="16"/>
+      <c r="J78" s="17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A79" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="B79" s="7">
+        <v>178</v>
+      </c>
+      <c r="C79" s="7"/>
+      <c r="D79" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="E79" s="7"/>
+      <c r="F79" s="7"/>
+      <c r="G79" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="H79" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="I79" s="14"/>
+      <c r="J79" s="15" t="s">
+        <v>76</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295"/>

</xml_diff>